<commit_message>
Informational and organizational update
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Licencja do Pycharma</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Uszkodzony układ audio u Piotera</t>
   </si>
@@ -35,13 +32,19 @@
     <t>Użyć nowych odzyskanych głośników</t>
   </si>
   <si>
-    <t>Uruchomić silniki krokowe</t>
-  </si>
-  <si>
-    <t>Prawdopodobnie przełożenie zębatek wymaga aktualizacji</t>
-  </si>
-  <si>
     <t>Poeksperymentować z trybami pracy driverów w silnikach</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Silniki krokowe</t>
+  </si>
+  <si>
+    <t>Przełożenie zębatek wymaga aktualizacji</t>
+  </si>
+  <si>
+    <t>Skonfigurować nową płytkę arduino+drv8825 zamiast ender3</t>
   </si>
 </sst>
 </file>
@@ -87,7 +90,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -372,47 +375,53 @@
   <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.28515625" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B5:B6"/>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ESP board initial setup
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Uszkodzony układ audio u Piotera</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Dodać głośnik basowy do pary</t>
+  </si>
+  <si>
+    <t>później</t>
+  </si>
+  <si>
+    <t>nie bardzo wiadomo jakiego przełożenia użyć - do sprawdzenia z realnym obciążeniem</t>
   </si>
 </sst>
 </file>
@@ -99,11 +105,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -114,7 +117,16 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,76 +408,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C9"/>
+  <dimension ref="B3:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="3" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="3" t="s">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
-      <c r="C4" s="2" t="s">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="1" t="s">
+      <c r="D9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
+      <c r="D10" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B7:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
improvements and cleanup for assembly
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Uszkodzony układ audio u Piotera</t>
   </si>
@@ -75,6 +75,27 @@
   </si>
   <si>
     <t>Przeprojektować model w inventorze, by obsługiwał silniki i Halla</t>
+  </si>
+  <si>
+    <t>zębatki wokół osi pionowej się rozjechały</t>
+  </si>
+  <si>
+    <t>constrainy na obrót wokół osi pionowej są zrąbane</t>
+  </si>
+  <si>
+    <t>czujniki hala na oś pionową i poziomą</t>
+  </si>
+  <si>
+    <t>miejsce na przewody ciśnieniowe</t>
+  </si>
+  <si>
+    <t>opcjonalnie: symulacja w inwentorze czy przełożenie jest ok</t>
+  </si>
+  <si>
+    <t>duża zębatki mogą być ucięte do połowy (180* ruchu zamiast 360*)</t>
+  </si>
+  <si>
+    <t>miejsce na płytkę raspbery i esp</t>
   </si>
 </sst>
 </file>
@@ -117,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -131,17 +152,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D14"/>
+  <dimension ref="B3:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,96 +461,142 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="2" t="s">
+      <c r="D8" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="7" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="1" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="2" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="B11:B14"/>
+  <mergeCells count="3">
+    <mergeCell ref="B3:B15"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C8:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
WIP: Inventor models for hal holders
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Uszkodzony układ audio u Piotera</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>miejsce na płytkę raspbery i esp</t>
+  </si>
+  <si>
+    <t>Przemyślenie prowadzenia kabli między komponentami</t>
+  </si>
+  <si>
+    <t>Obudowa</t>
+  </si>
+  <si>
+    <t>Siłowniki  i hydrostatyka</t>
+  </si>
+  <si>
+    <t>Kamera</t>
+  </si>
+  <si>
+    <t>Działka</t>
   </si>
 </sst>
 </file>
@@ -147,9 +162,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -158,14 +170,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,15 +462,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D20"/>
+  <dimension ref="B3:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="34.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" style="2" customWidth="1"/>
   </cols>
@@ -464,7 +479,7 @@
       <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -494,51 +509,51 @@
     </row>
     <row r="8" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
@@ -548,15 +563,15 @@
       <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -564,13 +579,13 @@
       <c r="B17" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -590,6 +605,29 @@
       </c>
       <c r="D20" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HAL sensors holders added to assembly
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -89,15 +89,9 @@
     <t>miejsce na przewody ciśnieniowe</t>
   </si>
   <si>
-    <t>opcjonalnie: symulacja w inwentorze czy przełożenie jest ok</t>
-  </si>
-  <si>
     <t>duża zębatki mogą być ucięte do połowy (180* ruchu zamiast 360*)</t>
   </si>
   <si>
-    <t>miejsce na płytkę raspbery i esp</t>
-  </si>
-  <si>
     <t>Przemyślenie prowadzenia kabli między komponentami</t>
   </si>
   <si>
@@ -111,6 +105,12 @@
   </si>
   <si>
     <t>Działka</t>
+  </si>
+  <si>
+    <t>PCB integrujące wszystkie płytki i komponenty</t>
+  </si>
+  <si>
+    <t>miejsce na płytki w modelu</t>
   </si>
 </sst>
 </file>
@@ -153,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -171,16 +171,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,14 +467,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -479,37 +482,37 @@
       <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -518,123 +521,122 @@
     </row>
     <row r="9" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
-      <c r="C11" s="6"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
-      <c r="C12" s="6"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>8</v>
+      <c r="B16" s="8"/>
+      <c r="C16" s="5" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>0</v>
+      <c r="B17" s="8"/>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
-      <c r="C18" s="5" t="s">
-        <v>1</v>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>11</v>
+      <c r="B19" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>11</v>
+      <c r="B20" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+    <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>24</v>
+      <c r="B24" s="8"/>
+      <c r="C24" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B3:B15"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="C8:C14"/>
+  <mergeCells count="4">
+    <mergeCell ref="B3:B13"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="B22:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>